<commit_message>
Updated Excel file with timestamp via Streamlit
</commit_message>
<xml_diff>
--- a/Generated_Responses.xlsx
+++ b/Generated_Responses.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Society</t>
   </si>
@@ -49,103 +49,43 @@
     <t>Name the Region where the society_name is from? Just name the US state or the Region in one word for the answer.</t>
   </si>
   <si>
+    <t>Last Updated</t>
+  </si>
+  <si>
     <t>Soleo Health</t>
   </si>
   <si>
-    <t>University of Miami</t>
-  </si>
-  <si>
-    <t>Dava Oncology, LP</t>
-  </si>
-  <si>
-    <t>500</t>
-  </si>
-  <si>
-    <t>25,000</t>
-  </si>
-  <si>
-    <t>160</t>
-  </si>
-  <si>
-    <t>No, Soleo Health does not encompass community sites. Soleo Health is a specialty pharmacy that primarily focuses on providing infusion therapy services rather than community-based healthcare.</t>
-  </si>
-  <si>
-    <t>No, the University of Miami society does not encompass community sites. Justification: It is primarily an educational institution.</t>
-  </si>
-  <si>
-    <t>no, Dava Oncology, LP is a limited partnership and not a society.</t>
-  </si>
-  <si>
-    <t>Yes, Soleo Health is influential on state and local policy. The company's size, scope of operations, and advocacy efforts within the healthcare sector contribute to its influence on policy decisions.</t>
-  </si>
-  <si>
-    <t>No, lack of direct evidence.</t>
-  </si>
-  <si>
-    <t>No, Dava Oncology, LP is not influential on state or local policy. The company is primarily focused on developing pharmaceuticals and hence does not have direct influence on policy decisions.</t>
-  </si>
-  <si>
-    <t>No, Soleo Health does not provide engagement opportunity with leadership. The company does not explicitly mention any leadership engagement initiatives for its society members.</t>
-  </si>
-  <si>
-    <t>Yes, The University of Miami provides engagement opportunities with leadership through various student organizations, leadership programs, and mentorship initiatives.</t>
-  </si>
-  <si>
-    <t>no, There is no direct evidence of leadership engagement opportunities provided by 'Dava Oncology, LP'.</t>
-  </si>
-  <si>
-    <t>No, Soleo Health does not provide support for clinical trial recruitment. Soleo Health primarily focuses on home infusion services and specialty pharmacy support.</t>
-  </si>
-  <si>
-    <t>Yes, justification: university's research focus.</t>
-  </si>
-  <si>
-    <t>yes, Dava Oncology, LP provides support for clinical trial recruitment. Dava Oncology, LP is known for its expertise in oncology clinical trial recruitment and provides dedicated services to support various clinical trials.</t>
-  </si>
-  <si>
-    <t>No, Soleo Health does not provide engagement opportunity with payors. Soleo Health is a specialty infusion services provider focusing on patient care rather than engaging directly with payors.</t>
-  </si>
-  <si>
-    <t>No, the University of Miami does not provide engagement opportunities with payors. This is because the primary focus of the university is on education and research, rather than engaging with payors for financial transactions.</t>
-  </si>
-  <si>
-    <t>No, Dava Oncology, LP does not provide engagement opportunities with payors. The reason is that it is a limited partnership and its structure may not involve direct engagement with payors.</t>
-  </si>
-  <si>
-    <t>Yes, Soleo Health includes area experts on its board. Area experts bring specialized knowledge and experience that can greatly benefit the organization in making informed decisions and strategic moves.</t>
-  </si>
-  <si>
-    <t>No, justification: The University of Miami does not have area experts on its board.</t>
-  </si>
-  <si>
-    <t>Yes, ,Dava Oncology, LP includes area experts on its board.</t>
-  </si>
-  <si>
-    <t>No, Soleo Health is not involved in therapeutic research collaborations. Justification: Soleo Health predominantly focuses on specialty infusion services rather than research collaborations.</t>
-  </si>
-  <si>
-    <t>Yes, University of Miami is involved in therapeutic research collaborations. The institution has robust partnerships with various organizations for advancing healthcare research and innovation.</t>
-  </si>
-  <si>
-    <t>No, as of our latest information, Dava Oncology, LP is not involved in therapeutic research collaborations.</t>
-  </si>
-  <si>
-    <t>No, as per the publicly available information, Soleo Health does not include top therapeutic area experts on its board.</t>
-  </si>
-  <si>
-    <t>No, the University of Miami does not include top therapeutic area experts on its board. The university's board typically consists of members with expertise in education, business, law, and various other fields related to university administration.</t>
-  </si>
-  <si>
-    <t>No, as per available information, Dava Oncology, LP does not include top therapeutic area experts on its board.</t>
+    <t>1500</t>
+  </si>
+  <si>
+    <t>No, Soleo Health does not encompass community sites. Soleo Health is a specialty pharmacy and infusion services provider focused on patient care in the home setting, rather than community sites.</t>
+  </si>
+  <si>
+    <t>No, Soleo Health is not influential on state or local policy. Soleo Health operates as a healthcare provider, focusing on specialty infusion services rather than advocacy or policy-making activities.</t>
+  </si>
+  <si>
+    <t>No, Soleo Health, The organization does not provide engagement opportunities with leadership. The company may lack transparency or structured programs to facilitate interactions with its leadership team.</t>
+  </si>
+  <si>
+    <t>No, Soleo Health does not provide support for clinical trial recruitment. Soleo Health focuses on specialty infusion services for patients.</t>
+  </si>
+  <si>
+    <t>No, Soleo Health does not provide engaging opportunities with payors. Payor engagement is not a prominent focus for Soleo Health.</t>
+  </si>
+  <si>
+    <t>No, Soleo Health does not include area experts on its board. The company primarily focuses on providing specialty infusion services and healthcare solutions rather than having industry-specific experts on its board of directors.</t>
+  </si>
+  <si>
+    <t>no, There is no public information available on therapeutic research collaborations involving Soleo Health.</t>
+  </si>
+  <si>
+    <t>No, justification: There is no public information available on the composition of Soleo Health's board to confirm if it includes top therapeutic area experts.</t>
   </si>
   <si>
     <t>Texas</t>
   </si>
   <si>
-    <t>Florida</t>
-  </si>
-  <si>
-    <t>The society "Dava Oncology, LP" is based in Texas.</t>
+    <t>2025-03-12 12:46:35</t>
   </si>
 </sst>
 </file>
@@ -503,13 +443,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -543,110 +483,46 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" t="s">
         <v>20</v>
       </c>
-      <c r="E2" t="s">
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" t="s">
         <v>23</v>
-      </c>
-      <c r="F2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I3" t="s">
-        <v>36</v>
-      </c>
-      <c r="J3" t="s">
-        <v>39</v>
-      </c>
-      <c r="K3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I4" t="s">
-        <v>37</v>
-      </c>
-      <c r="J4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K4" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>